<commit_message>
Resolve railway data discrepancies based on GIS analysis
Resolved 42 discrepancies through systematic review:
- 15 settlements updated to use GIS data
- 6 M&NW settlements confirmed (GIS lacks M&NW coverage)
- 20 settlements with no GIS coverage confirmed using original data
- 1 settlement (Denholm) flagged for research

11 entries remain for further research:
- Lebret, Macoun, Morse, Hudson Bay Jct, Sutherland (year differences)
- Rosthern (operator history)
- Weyburn, Warman, Pangman, Mazenod (railway verification)
- Lockwood (no data in either source)

Added Calculated_likelihood and Further_research_needed columns.

Note: Corresponding changes made to UrbanSaskHist_Update_Jan_2026.xlsx
in KnowledgeGraph folder (outside this repo).

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Historical_Railway_Data_By_Settlement.xlsx
+++ b/Historical_Railway_Data_By_Settlement.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I430"/>
+  <dimension ref="A1:J430"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,6 +479,11 @@
           <t>Calculated_likelihood</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Further_research_needed</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -495,18 +500,14 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>1888</v>
+        <v>1905</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>CPR, CNoR, GTPR</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Year: 1888 vs 1905 (+17); Missing in GIS: CPR</t>
-        </is>
-      </c>
+          <t>CNoR, GTPR</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr"/>
       <c r="G2" t="n">
         <v>1905</v>
       </c>
@@ -515,11 +516,8 @@
           <t>CNoR, GTPR</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>CPR: LOW - nearest line 34km away</t>
-        </is>
-      </c>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -553,6 +551,7 @@
         </is>
       </c>
       <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -573,14 +572,10 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>QLSRSC (first), CPR, CNoR, GTPR</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Missing in GIS: CPR</t>
-        </is>
-      </c>
+          <t>QLSRSC, CNoR, GTPR</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
       <c r="G4" t="n">
         <v>1890</v>
       </c>
@@ -589,11 +584,8 @@
           <t>QLSRSC, CNoR, GTPR</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>CPR: Operator confusion (Likely operator vs owner confusion)</t>
-        </is>
-      </c>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -610,18 +602,14 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>1882</v>
+        <v>1911</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>CPR, GTPR</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Year: 1882 vs 1911 (+29); Missing in GIS: CPR</t>
-        </is>
-      </c>
+          <t>GTPR</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
       <c r="G5" t="n">
         <v>1904</v>
       </c>
@@ -630,11 +618,8 @@
           <t>CPR, GTPR</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>CPR: MEDIUM - line 13km away</t>
-        </is>
-      </c>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -668,6 +653,7 @@
         </is>
       </c>
       <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -701,6 +687,7 @@
         </is>
       </c>
       <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -734,6 +721,7 @@
         </is>
       </c>
       <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -767,6 +755,7 @@
         </is>
       </c>
       <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -800,6 +789,7 @@
         </is>
       </c>
       <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -833,6 +823,7 @@
         </is>
       </c>
       <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -866,6 +857,7 @@
         </is>
       </c>
       <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -899,6 +891,7 @@
         </is>
       </c>
       <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -932,6 +925,7 @@
         </is>
       </c>
       <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -965,6 +959,7 @@
         </is>
       </c>
       <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -998,6 +993,7 @@
         </is>
       </c>
       <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1031,6 +1027,7 @@
         </is>
       </c>
       <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1064,6 +1061,7 @@
         </is>
       </c>
       <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1097,6 +1095,7 @@
         </is>
       </c>
       <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1130,6 +1129,7 @@
         </is>
       </c>
       <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1163,6 +1163,7 @@
         </is>
       </c>
       <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1196,6 +1197,7 @@
         </is>
       </c>
       <c r="I22" t="inlineStr"/>
+      <c r="J22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1229,6 +1231,7 @@
         </is>
       </c>
       <c r="I23" t="inlineStr"/>
+      <c r="J23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1262,6 +1265,7 @@
         </is>
       </c>
       <c r="I24" t="inlineStr"/>
+      <c r="J24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1282,12 +1286,12 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>M&amp;NW (first), CPR, GTPR, CN, CNoR</t>
+          <t>M&amp;NW (first), GTPR, CNoR</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Year: 1889 vs 1911 (+22); Missing in GIS: CPR, M&amp;NW</t>
+          <t>Resolved - M&amp;NW not in GIS, original data correct</t>
         </is>
       </c>
       <c r="G25" t="n">
@@ -1303,6 +1307,7 @@
           <t>CPR: VERY LOW - nearest line 57km away; M&amp;NW: HIGH - line 1km away, likely GIS gap</t>
         </is>
       </c>
+      <c r="J25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1336,6 +1341,7 @@
         </is>
       </c>
       <c r="I26" t="inlineStr"/>
+      <c r="J26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1369,6 +1375,7 @@
         </is>
       </c>
       <c r="I27" t="inlineStr"/>
+      <c r="J27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1402,6 +1409,7 @@
         </is>
       </c>
       <c r="I28" t="inlineStr"/>
+      <c r="J28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1435,6 +1443,7 @@
         </is>
       </c>
       <c r="I29" t="inlineStr"/>
+      <c r="J29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1468,6 +1477,7 @@
         </is>
       </c>
       <c r="I30" t="inlineStr"/>
+      <c r="J30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1501,6 +1511,7 @@
         </is>
       </c>
       <c r="I31" t="inlineStr"/>
+      <c r="J31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1534,6 +1545,7 @@
         </is>
       </c>
       <c r="I32" t="inlineStr"/>
+      <c r="J32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1567,6 +1579,7 @@
         </is>
       </c>
       <c r="I33" t="inlineStr"/>
+      <c r="J33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1600,6 +1613,7 @@
         </is>
       </c>
       <c r="I34" t="inlineStr"/>
+      <c r="J34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1616,7 +1630,7 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>1898</v>
+        <v>1882</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1625,7 +1639,7 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Year: 1898 vs 1882 (-16)</t>
+          <t>Resolved - using GIS data</t>
         </is>
       </c>
       <c r="G35" t="n">
@@ -1637,6 +1651,7 @@
         </is>
       </c>
       <c r="I35" t="inlineStr"/>
+      <c r="J35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1662,7 +1677,7 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Year: 1911 vs 1904 (-7)</t>
+          <t>Year: 1911 vs 1904 (+7)</t>
         </is>
       </c>
       <c r="G36" t="n">
@@ -1674,6 +1689,11 @@
         </is>
       </c>
       <c r="I36" t="inlineStr"/>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1691,7 +1711,11 @@
           <t>M&amp;NWR</t>
         </is>
       </c>
-      <c r="F37" t="inlineStr"/>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Resolved - M&amp;NW not in GIS, original data correct</t>
+        </is>
+      </c>
       <c r="G37" t="n">
         <v>1910</v>
       </c>
@@ -1701,6 +1725,7 @@
         </is>
       </c>
       <c r="I37" t="inlineStr"/>
+      <c r="J37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1734,6 +1759,7 @@
         </is>
       </c>
       <c r="I38" t="inlineStr"/>
+      <c r="J38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1767,6 +1793,7 @@
         </is>
       </c>
       <c r="I39" t="inlineStr"/>
+      <c r="J39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1800,6 +1827,7 @@
         </is>
       </c>
       <c r="I40" t="inlineStr"/>
+      <c r="J40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1833,6 +1861,7 @@
         </is>
       </c>
       <c r="I41" t="inlineStr"/>
+      <c r="J41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1850,10 +1879,15 @@
           <t>M&amp;NWR</t>
         </is>
       </c>
-      <c r="F42" t="inlineStr"/>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Resolved - M&amp;NW not in GIS, original data correct</t>
+        </is>
+      </c>
       <c r="G42" t="inlineStr"/>
       <c r="H42" t="inlineStr"/>
       <c r="I42" t="inlineStr"/>
+      <c r="J42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1887,6 +1921,7 @@
         </is>
       </c>
       <c r="I43" t="inlineStr"/>
+      <c r="J43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1920,6 +1955,7 @@
         </is>
       </c>
       <c r="I44" t="inlineStr"/>
+      <c r="J44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1937,10 +1973,15 @@
           <t>M&amp;NWR</t>
         </is>
       </c>
-      <c r="F45" t="inlineStr"/>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Resolved - M&amp;NW not in GIS, original data correct</t>
+        </is>
+      </c>
       <c r="G45" t="inlineStr"/>
       <c r="H45" t="inlineStr"/>
       <c r="I45" t="inlineStr"/>
+      <c r="J45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1974,6 +2015,7 @@
         </is>
       </c>
       <c r="I46" t="inlineStr"/>
+      <c r="J46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2007,6 +2049,7 @@
         </is>
       </c>
       <c r="I47" t="inlineStr"/>
+      <c r="J47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2040,6 +2083,7 @@
         </is>
       </c>
       <c r="I48" t="inlineStr"/>
+      <c r="J48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2073,6 +2117,7 @@
         </is>
       </c>
       <c r="I49" t="inlineStr"/>
+      <c r="J49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2090,10 +2135,15 @@
           <t>CPR (1903 or 1904, both dates given)</t>
         </is>
       </c>
-      <c r="F50" t="inlineStr"/>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Resolved - using original data (no GIS coverage)</t>
+        </is>
+      </c>
       <c r="G50" t="inlineStr"/>
       <c r="H50" t="inlineStr"/>
       <c r="I50" t="inlineStr"/>
+      <c r="J50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2127,6 +2177,7 @@
         </is>
       </c>
       <c r="I51" t="inlineStr"/>
+      <c r="J51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2160,6 +2211,7 @@
         </is>
       </c>
       <c r="I52" t="inlineStr"/>
+      <c r="J52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -2193,6 +2245,7 @@
         </is>
       </c>
       <c r="I53" t="inlineStr"/>
+      <c r="J53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -2226,6 +2279,7 @@
         </is>
       </c>
       <c r="I54" t="inlineStr"/>
+      <c r="J54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -2243,7 +2297,11 @@
           <t>M&amp;NWR</t>
         </is>
       </c>
-      <c r="F55" t="inlineStr"/>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Resolved - M&amp;NW not in GIS, original data correct</t>
+        </is>
+      </c>
       <c r="G55" t="n">
         <v>1915</v>
       </c>
@@ -2253,6 +2311,7 @@
         </is>
       </c>
       <c r="I55" t="inlineStr"/>
+      <c r="J55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -2278,7 +2337,7 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Missing in GIS: CNoR, CPR</t>
+          <t>Missing in GIS: CN, CNOR, CPR</t>
         </is>
       </c>
       <c r="G56" t="n">
@@ -2294,6 +2353,7 @@
           <t>CNoR: Operator confusion (CNoR took over QLSRSC line 1906); CPR: Operator confusion (CPR operated QLSRSC line 1896-1906)</t>
         </is>
       </c>
+      <c r="J56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2311,10 +2371,15 @@
           <t>CPR</t>
         </is>
       </c>
-      <c r="F57" t="inlineStr"/>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>Resolved - using original data (no GIS coverage)</t>
+        </is>
+      </c>
       <c r="G57" t="inlineStr"/>
       <c r="H57" t="inlineStr"/>
       <c r="I57" t="inlineStr"/>
+      <c r="J57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -2331,7 +2396,7 @@
         </is>
       </c>
       <c r="D58" t="n">
-        <v>1905</v>
+        <v>1892</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -2340,7 +2405,7 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>Year: 1905 vs 1892 (-13)</t>
+          <t>Resolved - GIS date, original railway context kept</t>
         </is>
       </c>
       <c r="G58" t="n">
@@ -2352,6 +2417,7 @@
         </is>
       </c>
       <c r="I58" t="inlineStr"/>
+      <c r="J58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -2385,6 +2451,7 @@
         </is>
       </c>
       <c r="I59" t="inlineStr"/>
+      <c r="J59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2418,6 +2485,7 @@
         </is>
       </c>
       <c r="I60" t="inlineStr"/>
+      <c r="J60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -2451,6 +2519,7 @@
         </is>
       </c>
       <c r="I61" t="inlineStr"/>
+      <c r="J61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -2484,6 +2553,7 @@
         </is>
       </c>
       <c r="I62" t="inlineStr"/>
+      <c r="J62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2517,6 +2587,7 @@
         </is>
       </c>
       <c r="I63" t="inlineStr"/>
+      <c r="J63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2550,6 +2621,7 @@
         </is>
       </c>
       <c r="I64" t="inlineStr"/>
+      <c r="J64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -2575,7 +2647,7 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>Missing in GIS: CNoR</t>
+          <t>Missing in GIS: CN, CNOR</t>
         </is>
       </c>
       <c r="G65" t="n">
@@ -2591,6 +2663,11 @@
           <t>CNoR: LOW - nearest line 30km away</t>
         </is>
       </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>Yes - verify railway data</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2624,6 +2701,7 @@
         </is>
       </c>
       <c r="I66" t="inlineStr"/>
+      <c r="J66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -2657,6 +2735,7 @@
         </is>
       </c>
       <c r="I67" t="inlineStr"/>
+      <c r="J67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -2690,6 +2769,7 @@
         </is>
       </c>
       <c r="I68" t="inlineStr"/>
+      <c r="J68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -2723,6 +2803,7 @@
         </is>
       </c>
       <c r="I69" t="inlineStr"/>
+      <c r="J69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -2756,6 +2837,7 @@
         </is>
       </c>
       <c r="I70" t="inlineStr"/>
+      <c r="J70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -2789,6 +2871,7 @@
         </is>
       </c>
       <c r="I71" t="inlineStr"/>
+      <c r="J71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -2822,6 +2905,7 @@
         </is>
       </c>
       <c r="I72" t="inlineStr"/>
+      <c r="J72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -2855,6 +2939,7 @@
         </is>
       </c>
       <c r="I73" t="inlineStr"/>
+      <c r="J73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -2871,16 +2956,16 @@
         </is>
       </c>
       <c r="D74" t="n">
-        <v>1901</v>
+        <v>1893</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>CPR (first)</t>
+          <t>CPR</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>Year: 1901 vs 1893 (-8)</t>
+          <t>Resolved - using GIS data</t>
         </is>
       </c>
       <c r="G74" t="n">
@@ -2892,6 +2977,7 @@
         </is>
       </c>
       <c r="I74" t="inlineStr"/>
+      <c r="J74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -2925,6 +3011,7 @@
         </is>
       </c>
       <c r="I75" t="inlineStr"/>
+      <c r="J75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -2958,6 +3045,7 @@
         </is>
       </c>
       <c r="I76" t="inlineStr"/>
+      <c r="J76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -2975,10 +3063,15 @@
           <t>CNoR</t>
         </is>
       </c>
-      <c r="F77" t="inlineStr"/>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>Resolved - using original data (no GIS coverage)</t>
+        </is>
+      </c>
       <c r="G77" t="inlineStr"/>
       <c r="H77" t="inlineStr"/>
       <c r="I77" t="inlineStr"/>
+      <c r="J77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -3012,6 +3105,7 @@
         </is>
       </c>
       <c r="I78" t="inlineStr"/>
+      <c r="J78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -3045,6 +3139,7 @@
         </is>
       </c>
       <c r="I79" t="inlineStr"/>
+      <c r="J79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -3078,6 +3173,7 @@
         </is>
       </c>
       <c r="I80" t="inlineStr"/>
+      <c r="J80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -3094,7 +3190,7 @@
         </is>
       </c>
       <c r="D81" t="n">
-        <v>1911</v>
+        <v>1905</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -3103,7 +3199,7 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>Year: 1911 vs 1905 (-6)</t>
+          <t>Resolved - using GIS data</t>
         </is>
       </c>
       <c r="G81" t="n">
@@ -3115,6 +3211,7 @@
         </is>
       </c>
       <c r="I81" t="inlineStr"/>
+      <c r="J81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -3148,6 +3245,7 @@
         </is>
       </c>
       <c r="I82" t="inlineStr"/>
+      <c r="J82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -3181,6 +3279,7 @@
         </is>
       </c>
       <c r="I83" t="inlineStr"/>
+      <c r="J83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -3214,6 +3313,7 @@
         </is>
       </c>
       <c r="I84" t="inlineStr"/>
+      <c r="J84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -3247,6 +3347,7 @@
         </is>
       </c>
       <c r="I85" t="inlineStr"/>
+      <c r="J85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -3280,6 +3381,7 @@
         </is>
       </c>
       <c r="I86" t="inlineStr"/>
+      <c r="J86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -3313,6 +3415,7 @@
         </is>
       </c>
       <c r="I87" t="inlineStr"/>
+      <c r="J87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -3346,6 +3449,7 @@
         </is>
       </c>
       <c r="I88" t="inlineStr"/>
+      <c r="J88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -3379,6 +3483,7 @@
         </is>
       </c>
       <c r="I89" t="inlineStr"/>
+      <c r="J89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -3395,7 +3500,7 @@
         </is>
       </c>
       <c r="D90" t="n">
-        <v>1902</v>
+        <v>1893</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -3404,7 +3509,7 @@
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>Year: 1902 vs 1893 (-9)</t>
+          <t>Resolved - using GIS data</t>
         </is>
       </c>
       <c r="G90" t="n">
@@ -3416,6 +3521,7 @@
         </is>
       </c>
       <c r="I90" t="inlineStr"/>
+      <c r="J90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -3449,6 +3555,7 @@
         </is>
       </c>
       <c r="I91" t="inlineStr"/>
+      <c r="J91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -3482,6 +3589,7 @@
         </is>
       </c>
       <c r="I92" t="inlineStr"/>
+      <c r="J92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -3515,6 +3623,7 @@
         </is>
       </c>
       <c r="I93" t="inlineStr"/>
+      <c r="J93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -3540,7 +3649,7 @@
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>Year: 1883 vs 1893 (+10)</t>
+          <t>Year: 1883 vs 1893 (-10)</t>
         </is>
       </c>
       <c r="G94" t="n">
@@ -3552,6 +3661,11 @@
         </is>
       </c>
       <c r="I94" t="inlineStr"/>
+      <c r="J94" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -3585,6 +3699,7 @@
         </is>
       </c>
       <c r="I95" t="inlineStr"/>
+      <c r="J95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -3618,6 +3733,7 @@
         </is>
       </c>
       <c r="I96" t="inlineStr"/>
+      <c r="J96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -3638,14 +3754,10 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>CNoR (first), CPR</t>
-        </is>
-      </c>
-      <c r="F97" t="inlineStr">
-        <is>
-          <t>Missing in GIS: CPR</t>
-        </is>
-      </c>
+          <t>CNoR</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr"/>
       <c r="G97" t="n">
         <v>1905</v>
       </c>
@@ -3654,11 +3766,8 @@
           <t>CNoR</t>
         </is>
       </c>
-      <c r="I97" t="inlineStr">
-        <is>
-          <t>CPR: VERY LOW - nearest line 88km away</t>
-        </is>
-      </c>
+      <c r="I97" t="inlineStr"/>
+      <c r="J97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -3675,18 +3784,14 @@
         </is>
       </c>
       <c r="D98" t="n">
-        <v>1903</v>
+        <v>1889</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>QLSRSC owned the line but CPR operated it</t>
-        </is>
-      </c>
-      <c r="F98" t="inlineStr">
-        <is>
-          <t>Year: 1903 vs 1889 (-14); Missing in GIS: CPR</t>
-        </is>
-      </c>
+          <t>QLSRSC</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr"/>
       <c r="G98" t="n">
         <v>1889</v>
       </c>
@@ -3695,11 +3800,8 @@
           <t>QLSRSC</t>
         </is>
       </c>
-      <c r="I98" t="inlineStr">
-        <is>
-          <t>CPR: Operator confusion (CPR operated QLSRSC line 1896-1906)</t>
-        </is>
-      </c>
+      <c r="I98" t="inlineStr"/>
+      <c r="J98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -3733,6 +3835,7 @@
         </is>
       </c>
       <c r="I99" t="inlineStr"/>
+      <c r="J99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -3749,16 +3852,16 @@
         </is>
       </c>
       <c r="D100" t="n">
-        <v>1911</v>
+        <v>1893</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>CNoR, CPR</t>
+          <t>CPR, CNoR</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>Year: 1911 vs 1893 (-18)</t>
+          <t>Resolved - using GIS data</t>
         </is>
       </c>
       <c r="G100" t="n">
@@ -3770,6 +3873,7 @@
         </is>
       </c>
       <c r="I100" t="inlineStr"/>
+      <c r="J100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -3803,6 +3907,7 @@
         </is>
       </c>
       <c r="I101" t="inlineStr"/>
+      <c r="J101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -3836,6 +3941,7 @@
         </is>
       </c>
       <c r="I102" t="inlineStr"/>
+      <c r="J102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -3869,6 +3975,7 @@
         </is>
       </c>
       <c r="I103" t="inlineStr"/>
+      <c r="J103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -3902,6 +4009,7 @@
         </is>
       </c>
       <c r="I104" t="inlineStr"/>
+      <c r="J104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -3935,6 +4043,7 @@
         </is>
       </c>
       <c r="I105" t="inlineStr"/>
+      <c r="J105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -3968,6 +4077,7 @@
         </is>
       </c>
       <c r="I106" t="inlineStr"/>
+      <c r="J106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -4001,6 +4111,7 @@
         </is>
       </c>
       <c r="I107" t="inlineStr"/>
+      <c r="J107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -4034,6 +4145,7 @@
         </is>
       </c>
       <c r="I108" t="inlineStr"/>
+      <c r="J108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -4067,6 +4179,7 @@
         </is>
       </c>
       <c r="I109" t="inlineStr"/>
+      <c r="J109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -4100,6 +4213,7 @@
         </is>
       </c>
       <c r="I110" t="inlineStr"/>
+      <c r="J110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -4133,6 +4247,7 @@
         </is>
       </c>
       <c r="I111" t="inlineStr"/>
+      <c r="J111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -4166,6 +4281,7 @@
         </is>
       </c>
       <c r="I112" t="inlineStr"/>
+      <c r="J112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -4199,6 +4315,7 @@
         </is>
       </c>
       <c r="I113" t="inlineStr"/>
+      <c r="J113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -4232,6 +4349,7 @@
         </is>
       </c>
       <c r="I114" t="inlineStr"/>
+      <c r="J114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -4265,6 +4383,7 @@
         </is>
       </c>
       <c r="I115" t="inlineStr"/>
+      <c r="J115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -4298,6 +4417,7 @@
         </is>
       </c>
       <c r="I116" t="inlineStr"/>
+      <c r="J116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -4331,6 +4451,7 @@
         </is>
       </c>
       <c r="I117" t="inlineStr"/>
+      <c r="J117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -4364,6 +4485,7 @@
         </is>
       </c>
       <c r="I118" t="inlineStr"/>
+      <c r="J118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -4380,7 +4502,7 @@
         </is>
       </c>
       <c r="D119" t="n">
-        <v>1904</v>
+        <v>1882</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -4389,7 +4511,7 @@
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>Year: 1904 vs 1882 (-22)</t>
+          <t>Resolved - using GIS data</t>
         </is>
       </c>
       <c r="G119" t="n">
@@ -4401,6 +4523,7 @@
         </is>
       </c>
       <c r="I119" t="inlineStr"/>
+      <c r="J119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -4434,6 +4557,7 @@
         </is>
       </c>
       <c r="I120" t="inlineStr"/>
+      <c r="J120" t="inlineStr"/>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -4467,6 +4591,7 @@
         </is>
       </c>
       <c r="I121" t="inlineStr"/>
+      <c r="J121" t="inlineStr"/>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -4500,6 +4625,7 @@
         </is>
       </c>
       <c r="I122" t="inlineStr"/>
+      <c r="J122" t="inlineStr"/>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -4533,6 +4659,7 @@
         </is>
       </c>
       <c r="I123" t="inlineStr"/>
+      <c r="J123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -4566,6 +4693,7 @@
         </is>
       </c>
       <c r="I124" t="inlineStr"/>
+      <c r="J124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -4586,14 +4714,10 @@
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>CPR, QLSRSC</t>
-        </is>
-      </c>
-      <c r="F125" t="inlineStr">
-        <is>
-          <t>Missing in GIS: CPR</t>
-        </is>
-      </c>
+          <t>QLSRSC</t>
+        </is>
+      </c>
+      <c r="F125" t="inlineStr"/>
       <c r="G125" t="n">
         <v>1889</v>
       </c>
@@ -4602,11 +4726,8 @@
           <t>QLSRSC</t>
         </is>
       </c>
-      <c r="I125" t="inlineStr">
-        <is>
-          <t>CPR: Operator confusion (Likely operator vs owner confusion)</t>
-        </is>
-      </c>
+      <c r="I125" t="inlineStr"/>
+      <c r="J125" t="inlineStr"/>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -4624,7 +4745,11 @@
           <t>CPR</t>
         </is>
       </c>
-      <c r="F126" t="inlineStr"/>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>Resolved - using original data (no GIS coverage)</t>
+        </is>
+      </c>
       <c r="G126" t="n">
         <v>1915</v>
       </c>
@@ -4634,6 +4759,7 @@
         </is>
       </c>
       <c r="I126" t="inlineStr"/>
+      <c r="J126" t="inlineStr"/>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -4667,6 +4793,7 @@
         </is>
       </c>
       <c r="I127" t="inlineStr"/>
+      <c r="J127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -4700,6 +4827,7 @@
         </is>
       </c>
       <c r="I128" t="inlineStr"/>
+      <c r="J128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -4733,6 +4861,7 @@
         </is>
       </c>
       <c r="I129" t="inlineStr"/>
+      <c r="J129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -4766,6 +4895,7 @@
         </is>
       </c>
       <c r="I130" t="inlineStr"/>
+      <c r="J130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -4799,6 +4929,7 @@
         </is>
       </c>
       <c r="I131" t="inlineStr"/>
+      <c r="J131" t="inlineStr"/>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -4832,6 +4963,7 @@
         </is>
       </c>
       <c r="I132" t="inlineStr"/>
+      <c r="J132" t="inlineStr"/>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -4865,6 +4997,7 @@
         </is>
       </c>
       <c r="I133" t="inlineStr"/>
+      <c r="J133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -4898,6 +5031,7 @@
         </is>
       </c>
       <c r="I134" t="inlineStr"/>
+      <c r="J134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -4931,6 +5065,7 @@
         </is>
       </c>
       <c r="I135" t="inlineStr"/>
+      <c r="J135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -4964,6 +5099,7 @@
         </is>
       </c>
       <c r="I136" t="inlineStr"/>
+      <c r="J136" t="inlineStr"/>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -4997,6 +5133,7 @@
         </is>
       </c>
       <c r="I137" t="inlineStr"/>
+      <c r="J137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -5030,6 +5167,7 @@
         </is>
       </c>
       <c r="I138" t="inlineStr"/>
+      <c r="J138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -5063,6 +5201,7 @@
         </is>
       </c>
       <c r="I139" t="inlineStr"/>
+      <c r="J139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -5096,6 +5235,7 @@
         </is>
       </c>
       <c r="I140" t="inlineStr"/>
+      <c r="J140" t="inlineStr"/>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -5129,6 +5269,7 @@
         </is>
       </c>
       <c r="I141" t="inlineStr"/>
+      <c r="J141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -5162,6 +5303,7 @@
         </is>
       </c>
       <c r="I142" t="inlineStr"/>
+      <c r="J142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -5195,6 +5337,7 @@
         </is>
       </c>
       <c r="I143" t="inlineStr"/>
+      <c r="J143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -5228,6 +5371,7 @@
         </is>
       </c>
       <c r="I144" t="inlineStr"/>
+      <c r="J144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -5261,6 +5405,7 @@
         </is>
       </c>
       <c r="I145" t="inlineStr"/>
+      <c r="J145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -5294,6 +5439,7 @@
         </is>
       </c>
       <c r="I146" t="inlineStr"/>
+      <c r="J146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -5327,6 +5473,7 @@
         </is>
       </c>
       <c r="I147" t="inlineStr"/>
+      <c r="J147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -5360,6 +5507,7 @@
         </is>
       </c>
       <c r="I148" t="inlineStr"/>
+      <c r="J148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -5393,6 +5541,7 @@
         </is>
       </c>
       <c r="I149" t="inlineStr"/>
+      <c r="J149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -5426,6 +5575,7 @@
         </is>
       </c>
       <c r="I150" t="inlineStr"/>
+      <c r="J150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -5442,7 +5592,7 @@
         </is>
       </c>
       <c r="D151" t="n">
-        <v>1908</v>
+        <v>1905</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -5451,7 +5601,7 @@
       </c>
       <c r="F151" t="inlineStr">
         <is>
-          <t>Year: 1908 vs 1905 (-3)</t>
+          <t>Resolved - using GIS data</t>
         </is>
       </c>
       <c r="G151" t="n">
@@ -5463,6 +5613,7 @@
         </is>
       </c>
       <c r="I151" t="inlineStr"/>
+      <c r="J151" t="inlineStr"/>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -5496,6 +5647,7 @@
         </is>
       </c>
       <c r="I152" t="inlineStr"/>
+      <c r="J152" t="inlineStr"/>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -5529,6 +5681,7 @@
         </is>
       </c>
       <c r="I153" t="inlineStr"/>
+      <c r="J153" t="inlineStr"/>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -5562,6 +5715,7 @@
         </is>
       </c>
       <c r="I154" t="inlineStr"/>
+      <c r="J154" t="inlineStr"/>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -5595,6 +5749,7 @@
         </is>
       </c>
       <c r="I155" t="inlineStr"/>
+      <c r="J155" t="inlineStr"/>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -5628,6 +5783,7 @@
         </is>
       </c>
       <c r="I156" t="inlineStr"/>
+      <c r="J156" t="inlineStr"/>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -5661,6 +5817,7 @@
         </is>
       </c>
       <c r="I157" t="inlineStr"/>
+      <c r="J157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -5694,6 +5851,7 @@
         </is>
       </c>
       <c r="I158" t="inlineStr"/>
+      <c r="J158" t="inlineStr"/>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -5727,6 +5885,7 @@
         </is>
       </c>
       <c r="I159" t="inlineStr"/>
+      <c r="J159" t="inlineStr"/>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -5760,6 +5919,7 @@
         </is>
       </c>
       <c r="I160" t="inlineStr"/>
+      <c r="J160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -5793,6 +5953,7 @@
         </is>
       </c>
       <c r="I161" t="inlineStr"/>
+      <c r="J161" t="inlineStr"/>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -5809,7 +5970,7 @@
         </is>
       </c>
       <c r="D162" t="n">
-        <v>1904</v>
+        <v>1882</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -5818,7 +5979,7 @@
       </c>
       <c r="F162" t="inlineStr">
         <is>
-          <t>Year: 1904 vs 1882 (-22)</t>
+          <t>Resolved - using GIS data</t>
         </is>
       </c>
       <c r="G162" t="n">
@@ -5830,6 +5991,7 @@
         </is>
       </c>
       <c r="I162" t="inlineStr"/>
+      <c r="J162" t="inlineStr"/>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -5863,6 +6025,7 @@
         </is>
       </c>
       <c r="I163" t="inlineStr"/>
+      <c r="J163" t="inlineStr"/>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -5896,6 +6059,7 @@
         </is>
       </c>
       <c r="I164" t="inlineStr"/>
+      <c r="J164" t="inlineStr"/>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -5913,10 +6077,15 @@
           <t>CPR</t>
         </is>
       </c>
-      <c r="F165" t="inlineStr"/>
+      <c r="F165" t="inlineStr">
+        <is>
+          <t>Resolved - using original data (no GIS coverage)</t>
+        </is>
+      </c>
       <c r="G165" t="inlineStr"/>
       <c r="H165" t="inlineStr"/>
       <c r="I165" t="inlineStr"/>
+      <c r="J165" t="inlineStr"/>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -5950,6 +6119,7 @@
         </is>
       </c>
       <c r="I166" t="inlineStr"/>
+      <c r="J166" t="inlineStr"/>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -5970,10 +6140,14 @@
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>GTPR (first), CN</t>
-        </is>
-      </c>
-      <c r="F167" t="inlineStr"/>
+          <t>GTPR</t>
+        </is>
+      </c>
+      <c r="F167" t="inlineStr">
+        <is>
+          <t>Resolved - using GIS data</t>
+        </is>
+      </c>
       <c r="G167" t="n">
         <v>1904</v>
       </c>
@@ -5983,6 +6157,7 @@
         </is>
       </c>
       <c r="I167" t="inlineStr"/>
+      <c r="J167" t="inlineStr"/>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -6016,6 +6191,7 @@
         </is>
       </c>
       <c r="I168" t="inlineStr"/>
+      <c r="J168" t="inlineStr"/>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -6049,6 +6225,7 @@
         </is>
       </c>
       <c r="I169" t="inlineStr"/>
+      <c r="J169" t="inlineStr"/>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -6082,6 +6259,7 @@
         </is>
       </c>
       <c r="I170" t="inlineStr"/>
+      <c r="J170" t="inlineStr"/>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -6115,6 +6293,7 @@
         </is>
       </c>
       <c r="I171" t="inlineStr"/>
+      <c r="J171" t="inlineStr"/>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -6148,6 +6327,7 @@
         </is>
       </c>
       <c r="I172" t="inlineStr"/>
+      <c r="J172" t="inlineStr"/>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -6181,6 +6361,7 @@
         </is>
       </c>
       <c r="I173" t="inlineStr"/>
+      <c r="J173" t="inlineStr"/>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -6214,6 +6395,7 @@
         </is>
       </c>
       <c r="I174" t="inlineStr"/>
+      <c r="J174" t="inlineStr"/>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -6247,6 +6429,7 @@
         </is>
       </c>
       <c r="I175" t="inlineStr"/>
+      <c r="J175" t="inlineStr"/>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -6280,6 +6463,7 @@
         </is>
       </c>
       <c r="I176" t="inlineStr"/>
+      <c r="J176" t="inlineStr"/>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -6313,6 +6497,7 @@
         </is>
       </c>
       <c r="I177" t="inlineStr"/>
+      <c r="J177" t="inlineStr"/>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -6346,6 +6531,7 @@
         </is>
       </c>
       <c r="I178" t="inlineStr"/>
+      <c r="J178" t="inlineStr"/>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -6379,6 +6565,7 @@
         </is>
       </c>
       <c r="I179" t="inlineStr"/>
+      <c r="J179" t="inlineStr"/>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -6412,6 +6599,7 @@
         </is>
       </c>
       <c r="I180" t="inlineStr"/>
+      <c r="J180" t="inlineStr"/>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -6437,7 +6625,7 @@
       </c>
       <c r="F181" t="inlineStr">
         <is>
-          <t>Year: 1902 vs 1890 (-12); Missing in GIS: CPR</t>
+          <t>Year: 1902 vs 1890 (+12); Missing in GIS: CPR</t>
         </is>
       </c>
       <c r="G181" t="n">
@@ -6453,6 +6641,11 @@
           <t>CPR: Operator confusion (CPR operated QLSRSC line 1896-1906)</t>
         </is>
       </c>
+      <c r="J181" t="inlineStr">
+        <is>
+          <t>Yes - verify railway data</t>
+        </is>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -6486,6 +6679,7 @@
         </is>
       </c>
       <c r="I182" t="inlineStr"/>
+      <c r="J182" t="inlineStr"/>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -6511,7 +6705,7 @@
       </c>
       <c r="F183" t="inlineStr">
         <is>
-          <t>Year: 1902 vs 1882 (-20)</t>
+          <t>Year: 1902 vs 1882 (+20)</t>
         </is>
       </c>
       <c r="G183" t="n">
@@ -6523,6 +6717,11 @@
         </is>
       </c>
       <c r="I183" t="inlineStr"/>
+      <c r="J183" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -6556,6 +6755,7 @@
         </is>
       </c>
       <c r="I184" t="inlineStr"/>
+      <c r="J184" t="inlineStr"/>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -6589,6 +6789,7 @@
         </is>
       </c>
       <c r="I185" t="inlineStr"/>
+      <c r="J185" t="inlineStr"/>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -6622,6 +6823,7 @@
         </is>
       </c>
       <c r="I186" t="inlineStr"/>
+      <c r="J186" t="inlineStr"/>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -6655,6 +6857,7 @@
         </is>
       </c>
       <c r="I187" t="inlineStr"/>
+      <c r="J187" t="inlineStr"/>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -6688,6 +6891,7 @@
         </is>
       </c>
       <c r="I188" t="inlineStr"/>
+      <c r="J188" t="inlineStr"/>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -6721,6 +6925,7 @@
         </is>
       </c>
       <c r="I189" t="inlineStr"/>
+      <c r="J189" t="inlineStr"/>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -6754,6 +6959,7 @@
         </is>
       </c>
       <c r="I190" t="inlineStr"/>
+      <c r="J190" t="inlineStr"/>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -6787,6 +6993,7 @@
         </is>
       </c>
       <c r="I191" t="inlineStr"/>
+      <c r="J191" t="inlineStr"/>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -6820,6 +7027,7 @@
         </is>
       </c>
       <c r="I192" t="inlineStr"/>
+      <c r="J192" t="inlineStr"/>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -6836,18 +7044,14 @@
         </is>
       </c>
       <c r="D193" t="n">
-        <v>1905</v>
+        <v>1908</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
-          <t>CNoR (later taken over by GTPR)</t>
-        </is>
-      </c>
-      <c r="F193" t="inlineStr">
-        <is>
-          <t>Year: 1905 vs 1908 (+3); Missing in GIS: CNoR</t>
-        </is>
-      </c>
+          <t>GTPR</t>
+        </is>
+      </c>
+      <c r="F193" t="inlineStr"/>
       <c r="G193" t="n">
         <v>1907</v>
       </c>
@@ -6856,11 +7060,8 @@
           <t>CPR, GTPR</t>
         </is>
       </c>
-      <c r="I193" t="inlineStr">
-        <is>
-          <t>CNoR: Operator confusion (CNoR line later operated by GTPR)</t>
-        </is>
-      </c>
+      <c r="I193" t="inlineStr"/>
+      <c r="J193" t="inlineStr"/>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -6877,16 +7078,16 @@
         </is>
       </c>
       <c r="D194" t="n">
-        <v>1908</v>
+        <v>1905</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
-          <t>CNoR was in Delmas by 1908, but may have come through earlier.</t>
+          <t>CNoR</t>
         </is>
       </c>
       <c r="F194" t="inlineStr">
         <is>
-          <t>Year: 1908 vs 1905 (-3)</t>
+          <t>Resolved - using GIS data</t>
         </is>
       </c>
       <c r="G194" t="n">
@@ -6898,6 +7099,7 @@
         </is>
       </c>
       <c r="I194" t="inlineStr"/>
+      <c r="J194" t="inlineStr"/>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -6915,10 +7117,15 @@
           <t>CNoR</t>
         </is>
       </c>
-      <c r="F195" t="inlineStr"/>
+      <c r="F195" t="inlineStr">
+        <is>
+          <t>Resolved - using original data (no GIS coverage)</t>
+        </is>
+      </c>
       <c r="G195" t="inlineStr"/>
       <c r="H195" t="inlineStr"/>
       <c r="I195" t="inlineStr"/>
+      <c r="J195" t="inlineStr"/>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -6952,6 +7159,7 @@
         </is>
       </c>
       <c r="I196" t="inlineStr"/>
+      <c r="J196" t="inlineStr"/>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -6985,6 +7193,7 @@
         </is>
       </c>
       <c r="I197" t="inlineStr"/>
+      <c r="J197" t="inlineStr"/>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -7018,6 +7227,7 @@
         </is>
       </c>
       <c r="I198" t="inlineStr"/>
+      <c r="J198" t="inlineStr"/>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -7051,6 +7261,7 @@
         </is>
       </c>
       <c r="I199" t="inlineStr"/>
+      <c r="J199" t="inlineStr"/>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -7084,6 +7295,7 @@
         </is>
       </c>
       <c r="I200" t="inlineStr"/>
+      <c r="J200" t="inlineStr"/>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
@@ -7117,6 +7329,7 @@
         </is>
       </c>
       <c r="I201" t="inlineStr"/>
+      <c r="J201" t="inlineStr"/>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -7150,6 +7363,7 @@
         </is>
       </c>
       <c r="I202" t="inlineStr"/>
+      <c r="J202" t="inlineStr"/>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
@@ -7175,7 +7389,7 @@
       </c>
       <c r="F203" t="inlineStr">
         <is>
-          <t>Year: 1913 vs 1905 (-8)</t>
+          <t>Resolved - using original data</t>
         </is>
       </c>
       <c r="G203" t="n">
@@ -7187,6 +7401,11 @@
         </is>
       </c>
       <c r="I203" t="inlineStr"/>
+      <c r="J203" t="inlineStr">
+        <is>
+          <t>Yes - GIS data seems wrong</t>
+        </is>
+      </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
@@ -7220,6 +7439,7 @@
         </is>
       </c>
       <c r="I204" t="inlineStr"/>
+      <c r="J204" t="inlineStr"/>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
@@ -7253,6 +7473,7 @@
         </is>
       </c>
       <c r="I205" t="inlineStr"/>
+      <c r="J205" t="inlineStr"/>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
@@ -7286,6 +7507,7 @@
         </is>
       </c>
       <c r="I206" t="inlineStr"/>
+      <c r="J206" t="inlineStr"/>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
@@ -7319,6 +7541,7 @@
         </is>
       </c>
       <c r="I207" t="inlineStr"/>
+      <c r="J207" t="inlineStr"/>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
@@ -7336,10 +7559,15 @@
           <t>M&amp;NWR</t>
         </is>
       </c>
-      <c r="F208" t="inlineStr"/>
+      <c r="F208" t="inlineStr">
+        <is>
+          <t>Resolved - M&amp;NW not in GIS, original data correct</t>
+        </is>
+      </c>
       <c r="G208" t="inlineStr"/>
       <c r="H208" t="inlineStr"/>
       <c r="I208" t="inlineStr"/>
+      <c r="J208" t="inlineStr"/>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
@@ -7373,6 +7601,7 @@
         </is>
       </c>
       <c r="I209" t="inlineStr"/>
+      <c r="J209" t="inlineStr"/>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
@@ -7406,6 +7635,7 @@
         </is>
       </c>
       <c r="I210" t="inlineStr"/>
+      <c r="J210" t="inlineStr"/>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
@@ -7439,6 +7669,7 @@
         </is>
       </c>
       <c r="I211" t="inlineStr"/>
+      <c r="J211" t="inlineStr"/>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
@@ -7472,6 +7703,7 @@
         </is>
       </c>
       <c r="I212" t="inlineStr"/>
+      <c r="J212" t="inlineStr"/>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
@@ -7505,6 +7737,7 @@
         </is>
       </c>
       <c r="I213" t="inlineStr"/>
+      <c r="J213" t="inlineStr"/>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
@@ -7538,6 +7771,7 @@
         </is>
       </c>
       <c r="I214" t="inlineStr"/>
+      <c r="J214" t="inlineStr"/>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
@@ -7571,6 +7805,7 @@
         </is>
       </c>
       <c r="I215" t="inlineStr"/>
+      <c r="J215" t="inlineStr"/>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
@@ -7604,6 +7839,7 @@
         </is>
       </c>
       <c r="I216" t="inlineStr"/>
+      <c r="J216" t="inlineStr"/>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
@@ -7637,6 +7873,7 @@
         </is>
       </c>
       <c r="I217" t="inlineStr"/>
+      <c r="J217" t="inlineStr"/>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
@@ -7670,6 +7907,7 @@
         </is>
       </c>
       <c r="I218" t="inlineStr"/>
+      <c r="J218" t="inlineStr"/>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
@@ -7703,6 +7941,7 @@
         </is>
       </c>
       <c r="I219" t="inlineStr"/>
+      <c r="J219" t="inlineStr"/>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
@@ -7736,6 +7975,7 @@
         </is>
       </c>
       <c r="I220" t="inlineStr"/>
+      <c r="J220" t="inlineStr"/>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
@@ -7769,6 +8009,7 @@
         </is>
       </c>
       <c r="I221" t="inlineStr"/>
+      <c r="J221" t="inlineStr"/>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
@@ -7802,6 +8043,7 @@
         </is>
       </c>
       <c r="I222" t="inlineStr"/>
+      <c r="J222" t="inlineStr"/>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
@@ -7835,6 +8077,7 @@
         </is>
       </c>
       <c r="I223" t="inlineStr"/>
+      <c r="J223" t="inlineStr"/>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
@@ -7868,6 +8111,7 @@
         </is>
       </c>
       <c r="I224" t="inlineStr"/>
+      <c r="J224" t="inlineStr"/>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
@@ -7901,6 +8145,7 @@
         </is>
       </c>
       <c r="I225" t="inlineStr"/>
+      <c r="J225" t="inlineStr"/>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
@@ -7918,10 +8163,15 @@
           <t>CPR</t>
         </is>
       </c>
-      <c r="F226" t="inlineStr"/>
+      <c r="F226" t="inlineStr">
+        <is>
+          <t>Resolved - using original data (no GIS coverage)</t>
+        </is>
+      </c>
       <c r="G226" t="inlineStr"/>
       <c r="H226" t="inlineStr"/>
       <c r="I226" t="inlineStr"/>
+      <c r="J226" t="inlineStr"/>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
@@ -7955,6 +8205,7 @@
         </is>
       </c>
       <c r="I227" t="inlineStr"/>
+      <c r="J227" t="inlineStr"/>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
@@ -7988,6 +8239,7 @@
         </is>
       </c>
       <c r="I228" t="inlineStr"/>
+      <c r="J228" t="inlineStr"/>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
@@ -8008,14 +8260,10 @@
       </c>
       <c r="E229" t="inlineStr">
         <is>
-          <t>CNoR, GTPR</t>
-        </is>
-      </c>
-      <c r="F229" t="inlineStr">
-        <is>
-          <t>Missing in GIS: CNoR</t>
-        </is>
-      </c>
+          <t>GTPR</t>
+        </is>
+      </c>
+      <c r="F229" t="inlineStr"/>
       <c r="G229" t="n">
         <v>1909</v>
       </c>
@@ -8024,11 +8272,8 @@
           <t>CPR, GTPR</t>
         </is>
       </c>
-      <c r="I229" t="inlineStr">
-        <is>
-          <t>CNoR: VERY LOW - nearest line 41km away</t>
-        </is>
-      </c>
+      <c r="I229" t="inlineStr"/>
+      <c r="J229" t="inlineStr"/>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
@@ -8049,14 +8294,10 @@
       </c>
       <c r="E230" t="inlineStr">
         <is>
-          <t>CNoR, CPR</t>
-        </is>
-      </c>
-      <c r="F230" t="inlineStr">
-        <is>
-          <t>Missing in GIS: CNoR</t>
-        </is>
-      </c>
+          <t>CPR</t>
+        </is>
+      </c>
+      <c r="F230" t="inlineStr"/>
       <c r="G230" t="n">
         <v>1908</v>
       </c>
@@ -8065,11 +8306,8 @@
           <t>CNoR, CPR</t>
         </is>
       </c>
-      <c r="I230" t="inlineStr">
-        <is>
-          <t>CNoR: MEDIUM - line 12km away</t>
-        </is>
-      </c>
+      <c r="I230" t="inlineStr"/>
+      <c r="J230" t="inlineStr"/>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
@@ -8103,6 +8341,7 @@
         </is>
       </c>
       <c r="I231" t="inlineStr"/>
+      <c r="J231" t="inlineStr"/>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
@@ -8123,14 +8362,10 @@
       </c>
       <c r="E232" t="inlineStr">
         <is>
-          <t>CNoR, GTPR</t>
-        </is>
-      </c>
-      <c r="F232" t="inlineStr">
-        <is>
-          <t>Missing in GIS: CNoR</t>
-        </is>
-      </c>
+          <t>GTPR</t>
+        </is>
+      </c>
+      <c r="F232" t="inlineStr"/>
       <c r="G232" t="n">
         <v>1908</v>
       </c>
@@ -8139,11 +8374,8 @@
           <t>CPR, GTPR</t>
         </is>
       </c>
-      <c r="I232" t="inlineStr">
-        <is>
-          <t>CNoR: VERY LOW - nearest line 51km away</t>
-        </is>
-      </c>
+      <c r="I232" t="inlineStr"/>
+      <c r="J232" t="inlineStr"/>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
@@ -8169,7 +8401,7 @@
       </c>
       <c r="F233" t="inlineStr">
         <is>
-          <t>Year: 1910 vs 1905 (-5)</t>
+          <t>Year: 1910 vs 1905 (+5)</t>
         </is>
       </c>
       <c r="G233" t="n">
@@ -8181,6 +8413,11 @@
         </is>
       </c>
       <c r="I233" t="inlineStr"/>
+      <c r="J233" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
@@ -8214,6 +8451,7 @@
         </is>
       </c>
       <c r="I234" t="inlineStr"/>
+      <c r="J234" t="inlineStr"/>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
@@ -8247,6 +8485,7 @@
         </is>
       </c>
       <c r="I235" t="inlineStr"/>
+      <c r="J235" t="inlineStr"/>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
@@ -8280,6 +8519,7 @@
         </is>
       </c>
       <c r="I236" t="inlineStr"/>
+      <c r="J236" t="inlineStr"/>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
@@ -8313,6 +8553,7 @@
         </is>
       </c>
       <c r="I237" t="inlineStr"/>
+      <c r="J237" t="inlineStr"/>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
@@ -8346,6 +8587,7 @@
         </is>
       </c>
       <c r="I238" t="inlineStr"/>
+      <c r="J238" t="inlineStr"/>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
@@ -8379,6 +8621,7 @@
         </is>
       </c>
       <c r="I239" t="inlineStr"/>
+      <c r="J239" t="inlineStr"/>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
@@ -8412,6 +8655,7 @@
         </is>
       </c>
       <c r="I240" t="inlineStr"/>
+      <c r="J240" t="inlineStr"/>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
@@ -8445,6 +8689,7 @@
         </is>
       </c>
       <c r="I241" t="inlineStr"/>
+      <c r="J241" t="inlineStr"/>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
@@ -8478,6 +8723,7 @@
         </is>
       </c>
       <c r="I242" t="inlineStr"/>
+      <c r="J242" t="inlineStr"/>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
@@ -8511,6 +8757,7 @@
         </is>
       </c>
       <c r="I243" t="inlineStr"/>
+      <c r="J243" t="inlineStr"/>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
@@ -8527,7 +8774,7 @@
         </is>
       </c>
       <c r="D244" t="n">
-        <v>1905</v>
+        <v>1882</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -8536,7 +8783,7 @@
       </c>
       <c r="F244" t="inlineStr">
         <is>
-          <t>Year: 1905 vs 1882 (-23)</t>
+          <t>Resolved - using GIS data</t>
         </is>
       </c>
       <c r="G244" t="n">
@@ -8548,6 +8795,7 @@
         </is>
       </c>
       <c r="I244" t="inlineStr"/>
+      <c r="J244" t="inlineStr"/>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
@@ -8581,6 +8829,7 @@
         </is>
       </c>
       <c r="I245" t="inlineStr"/>
+      <c r="J245" t="inlineStr"/>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
@@ -8614,6 +8863,7 @@
         </is>
       </c>
       <c r="I246" t="inlineStr"/>
+      <c r="J246" t="inlineStr"/>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
@@ -8647,6 +8897,7 @@
         </is>
       </c>
       <c r="I247" t="inlineStr"/>
+      <c r="J247" t="inlineStr"/>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
@@ -8680,6 +8931,7 @@
         </is>
       </c>
       <c r="I248" t="inlineStr"/>
+      <c r="J248" t="inlineStr"/>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
@@ -8713,6 +8965,7 @@
         </is>
       </c>
       <c r="I249" t="inlineStr"/>
+      <c r="J249" t="inlineStr"/>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
@@ -8746,6 +8999,7 @@
         </is>
       </c>
       <c r="I250" t="inlineStr"/>
+      <c r="J250" t="inlineStr"/>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
@@ -8779,6 +9033,7 @@
         </is>
       </c>
       <c r="I251" t="inlineStr"/>
+      <c r="J251" t="inlineStr"/>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
@@ -8812,6 +9067,7 @@
         </is>
       </c>
       <c r="I252" t="inlineStr"/>
+      <c r="J252" t="inlineStr"/>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
@@ -8845,6 +9101,7 @@
         </is>
       </c>
       <c r="I253" t="inlineStr"/>
+      <c r="J253" t="inlineStr"/>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
@@ -8862,7 +9119,11 @@
           <t>CPR</t>
         </is>
       </c>
-      <c r="F254" t="inlineStr"/>
+      <c r="F254" t="inlineStr">
+        <is>
+          <t>Resolved - using original data (no GIS coverage)</t>
+        </is>
+      </c>
       <c r="G254" t="n">
         <v>1921</v>
       </c>
@@ -8872,6 +9133,7 @@
         </is>
       </c>
       <c r="I254" t="inlineStr"/>
+      <c r="J254" t="inlineStr"/>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
@@ -8905,6 +9167,7 @@
         </is>
       </c>
       <c r="I255" t="inlineStr"/>
+      <c r="J255" t="inlineStr"/>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
@@ -8938,6 +9201,7 @@
         </is>
       </c>
       <c r="I256" t="inlineStr"/>
+      <c r="J256" t="inlineStr"/>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
@@ -8963,7 +9227,7 @@
       </c>
       <c r="F257" t="inlineStr">
         <is>
-          <t>Year: 1908 vs 1889 (-19)</t>
+          <t>Year: 1908 vs 1889 (+19)</t>
         </is>
       </c>
       <c r="G257" t="n">
@@ -8975,6 +9239,11 @@
         </is>
       </c>
       <c r="I257" t="inlineStr"/>
+      <c r="J257" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
@@ -9008,6 +9277,7 @@
         </is>
       </c>
       <c r="I258" t="inlineStr"/>
+      <c r="J258" t="inlineStr"/>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
@@ -9041,6 +9311,7 @@
         </is>
       </c>
       <c r="I259" t="inlineStr"/>
+      <c r="J259" t="inlineStr"/>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
@@ -9074,6 +9345,7 @@
         </is>
       </c>
       <c r="I260" t="inlineStr"/>
+      <c r="J260" t="inlineStr"/>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
@@ -9094,14 +9366,10 @@
       </c>
       <c r="E261" t="inlineStr">
         <is>
-          <t>CPR, QLSRSC</t>
-        </is>
-      </c>
-      <c r="F261" t="inlineStr">
-        <is>
-          <t>Missing in GIS: CPR</t>
-        </is>
-      </c>
+          <t>QLSRSC</t>
+        </is>
+      </c>
+      <c r="F261" t="inlineStr"/>
       <c r="G261" t="n">
         <v>1889</v>
       </c>
@@ -9110,11 +9378,8 @@
           <t>QLSRSC, CPR</t>
         </is>
       </c>
-      <c r="I261" t="inlineStr">
-        <is>
-          <t>CPR: Operator confusion (Likely operator vs owner confusion)</t>
-        </is>
-      </c>
+      <c r="I261" t="inlineStr"/>
+      <c r="J261" t="inlineStr"/>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
@@ -9148,6 +9413,7 @@
         </is>
       </c>
       <c r="I262" t="inlineStr"/>
+      <c r="J262" t="inlineStr"/>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
@@ -9181,6 +9447,7 @@
         </is>
       </c>
       <c r="I263" t="inlineStr"/>
+      <c r="J263" t="inlineStr"/>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
@@ -9198,10 +9465,15 @@
           <t>CNoR</t>
         </is>
       </c>
-      <c r="F264" t="inlineStr"/>
+      <c r="F264" t="inlineStr">
+        <is>
+          <t>Resolved - using original data (no GIS coverage)</t>
+        </is>
+      </c>
       <c r="G264" t="inlineStr"/>
       <c r="H264" t="inlineStr"/>
       <c r="I264" t="inlineStr"/>
+      <c r="J264" t="inlineStr"/>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
@@ -9235,6 +9507,7 @@
         </is>
       </c>
       <c r="I265" t="inlineStr"/>
+      <c r="J265" t="inlineStr"/>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
@@ -9268,6 +9541,7 @@
         </is>
       </c>
       <c r="I266" t="inlineStr"/>
+      <c r="J266" t="inlineStr"/>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
@@ -9301,6 +9575,7 @@
         </is>
       </c>
       <c r="I267" t="inlineStr"/>
+      <c r="J267" t="inlineStr"/>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
@@ -9334,6 +9609,7 @@
         </is>
       </c>
       <c r="I268" t="inlineStr"/>
+      <c r="J268" t="inlineStr"/>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
@@ -9367,6 +9643,7 @@
         </is>
       </c>
       <c r="I269" t="inlineStr"/>
+      <c r="J269" t="inlineStr"/>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
@@ -9400,6 +9677,7 @@
         </is>
       </c>
       <c r="I270" t="inlineStr"/>
+      <c r="J270" t="inlineStr"/>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
@@ -9433,6 +9711,7 @@
         </is>
       </c>
       <c r="I271" t="inlineStr"/>
+      <c r="J271" t="inlineStr"/>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
@@ -9450,10 +9729,15 @@
           <t>CN (Canadian National Railway)</t>
         </is>
       </c>
-      <c r="F272" t="inlineStr"/>
+      <c r="F272" t="inlineStr">
+        <is>
+          <t>Resolved - using original data (no GIS coverage)</t>
+        </is>
+      </c>
       <c r="G272" t="inlineStr"/>
       <c r="H272" t="inlineStr"/>
       <c r="I272" t="inlineStr"/>
+      <c r="J272" t="inlineStr"/>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
@@ -9465,7 +9749,11 @@
       <c r="C273" t="inlineStr"/>
       <c r="D273" t="inlineStr"/>
       <c r="E273" t="inlineStr"/>
-      <c r="F273" t="inlineStr"/>
+      <c r="F273" t="inlineStr">
+        <is>
+          <t>No data in either source</t>
+        </is>
+      </c>
       <c r="G273" t="n">
         <v>1907</v>
       </c>
@@ -9475,6 +9763,7 @@
         </is>
       </c>
       <c r="I273" t="inlineStr"/>
+      <c r="J273" t="inlineStr"/>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
@@ -9508,6 +9797,7 @@
         </is>
       </c>
       <c r="I274" t="inlineStr"/>
+      <c r="J274" t="inlineStr"/>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
@@ -9541,6 +9831,7 @@
         </is>
       </c>
       <c r="I275" t="inlineStr"/>
+      <c r="J275" t="inlineStr"/>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
@@ -9574,6 +9865,7 @@
         </is>
       </c>
       <c r="I276" t="inlineStr"/>
+      <c r="J276" t="inlineStr"/>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
@@ -9607,6 +9899,7 @@
         </is>
       </c>
       <c r="I277" t="inlineStr"/>
+      <c r="J277" t="inlineStr"/>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
@@ -9640,6 +9933,7 @@
         </is>
       </c>
       <c r="I278" t="inlineStr"/>
+      <c r="J278" t="inlineStr"/>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
@@ -9657,10 +9951,15 @@
           <t>CPR</t>
         </is>
       </c>
-      <c r="F279" t="inlineStr"/>
+      <c r="F279" t="inlineStr">
+        <is>
+          <t>Resolved - using original data (no GIS coverage)</t>
+        </is>
+      </c>
       <c r="G279" t="inlineStr"/>
       <c r="H279" t="inlineStr"/>
       <c r="I279" t="inlineStr"/>
+      <c r="J279" t="inlineStr"/>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
@@ -9694,6 +9993,7 @@
         </is>
       </c>
       <c r="I280" t="inlineStr"/>
+      <c r="J280" t="inlineStr"/>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
@@ -9727,6 +10027,7 @@
         </is>
       </c>
       <c r="I281" t="inlineStr"/>
+      <c r="J281" t="inlineStr"/>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
@@ -9760,6 +10061,7 @@
         </is>
       </c>
       <c r="I282" t="inlineStr"/>
+      <c r="J282" t="inlineStr"/>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
@@ -9793,6 +10095,7 @@
         </is>
       </c>
       <c r="I283" t="inlineStr"/>
+      <c r="J283" t="inlineStr"/>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
@@ -9826,6 +10129,7 @@
         </is>
       </c>
       <c r="I284" t="inlineStr"/>
+      <c r="J284" t="inlineStr"/>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
@@ -9859,6 +10163,7 @@
         </is>
       </c>
       <c r="I285" t="inlineStr"/>
+      <c r="J285" t="inlineStr"/>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
@@ -9879,14 +10184,10 @@
       </c>
       <c r="E286" t="inlineStr">
         <is>
-          <t>CNoR, GTPR</t>
-        </is>
-      </c>
-      <c r="F286" t="inlineStr">
-        <is>
-          <t>Missing in GIS: CNoR</t>
-        </is>
-      </c>
+          <t>GTPR</t>
+        </is>
+      </c>
+      <c r="F286" t="inlineStr"/>
       <c r="G286" t="n">
         <v>1908</v>
       </c>
@@ -9895,11 +10196,8 @@
           <t>GTPR</t>
         </is>
       </c>
-      <c r="I286" t="inlineStr">
-        <is>
-          <t>CNoR: VERY LOW - nearest line 72km away</t>
-        </is>
-      </c>
+      <c r="I286" t="inlineStr"/>
+      <c r="J286" t="inlineStr"/>
     </row>
     <row r="287">
       <c r="A287" t="inlineStr">
@@ -9933,6 +10231,7 @@
         </is>
       </c>
       <c r="I287" t="inlineStr"/>
+      <c r="J287" t="inlineStr"/>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
@@ -9966,6 +10265,7 @@
         </is>
       </c>
       <c r="I288" t="inlineStr"/>
+      <c r="J288" t="inlineStr"/>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">
@@ -9999,6 +10299,7 @@
         </is>
       </c>
       <c r="I289" t="inlineStr"/>
+      <c r="J289" t="inlineStr"/>
     </row>
     <row r="290">
       <c r="A290" t="inlineStr">
@@ -10032,6 +10333,7 @@
         </is>
       </c>
       <c r="I290" t="inlineStr"/>
+      <c r="J290" t="inlineStr"/>
     </row>
     <row r="291">
       <c r="A291" t="inlineStr">
@@ -10065,6 +10367,7 @@
         </is>
       </c>
       <c r="I291" t="inlineStr"/>
+      <c r="J291" t="inlineStr"/>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">
@@ -10098,6 +10401,7 @@
         </is>
       </c>
       <c r="I292" t="inlineStr"/>
+      <c r="J292" t="inlineStr"/>
     </row>
     <row r="293">
       <c r="A293" t="inlineStr">
@@ -10131,6 +10435,7 @@
         </is>
       </c>
       <c r="I293" t="inlineStr"/>
+      <c r="J293" t="inlineStr"/>
     </row>
     <row r="294">
       <c r="A294" t="inlineStr">
@@ -10164,6 +10469,7 @@
         </is>
       </c>
       <c r="I294" t="inlineStr"/>
+      <c r="J294" t="inlineStr"/>
     </row>
     <row r="295">
       <c r="A295" t="inlineStr">
@@ -10197,6 +10503,7 @@
         </is>
       </c>
       <c r="I295" t="inlineStr"/>
+      <c r="J295" t="inlineStr"/>
     </row>
     <row r="296">
       <c r="A296" t="inlineStr">
@@ -10236,6 +10543,11 @@
       <c r="I296" t="inlineStr">
         <is>
           <t>CPR: MEDIUM - line 11km away</t>
+        </is>
+      </c>
+      <c r="J296" t="inlineStr">
+        <is>
+          <t>Yes - verify railway data</t>
         </is>
       </c>
     </row>
@@ -10271,6 +10583,7 @@
         </is>
       </c>
       <c r="I297" t="inlineStr"/>
+      <c r="J297" t="inlineStr"/>
     </row>
     <row r="298">
       <c r="A298" t="inlineStr">
@@ -10304,6 +10617,7 @@
         </is>
       </c>
       <c r="I298" t="inlineStr"/>
+      <c r="J298" t="inlineStr"/>
     </row>
     <row r="299">
       <c r="A299" t="inlineStr">
@@ -10343,6 +10657,11 @@
       <c r="I299" t="inlineStr">
         <is>
           <t>CPR: MEDIUM - line 12km away</t>
+        </is>
+      </c>
+      <c r="J299" t="inlineStr">
+        <is>
+          <t>Yes - verify railway data</t>
         </is>
       </c>
     </row>
@@ -10362,10 +10681,15 @@
           <t>CNoR</t>
         </is>
       </c>
-      <c r="F300" t="inlineStr"/>
+      <c r="F300" t="inlineStr">
+        <is>
+          <t>Resolved - using original data (no GIS coverage)</t>
+        </is>
+      </c>
       <c r="G300" t="inlineStr"/>
       <c r="H300" t="inlineStr"/>
       <c r="I300" t="inlineStr"/>
+      <c r="J300" t="inlineStr"/>
     </row>
     <row r="301">
       <c r="A301" t="inlineStr">
@@ -10399,6 +10723,7 @@
         </is>
       </c>
       <c r="I301" t="inlineStr"/>
+      <c r="J301" t="inlineStr"/>
     </row>
     <row r="302">
       <c r="A302" t="inlineStr">
@@ -10432,6 +10757,7 @@
         </is>
       </c>
       <c r="I302" t="inlineStr"/>
+      <c r="J302" t="inlineStr"/>
     </row>
     <row r="303">
       <c r="A303" t="inlineStr">
@@ -10465,6 +10791,7 @@
         </is>
       </c>
       <c r="I303" t="inlineStr"/>
+      <c r="J303" t="inlineStr"/>
     </row>
     <row r="304">
       <c r="A304" t="inlineStr">
@@ -10498,6 +10825,7 @@
         </is>
       </c>
       <c r="I304" t="inlineStr"/>
+      <c r="J304" t="inlineStr"/>
     </row>
     <row r="305">
       <c r="A305" t="inlineStr">
@@ -10531,6 +10859,7 @@
         </is>
       </c>
       <c r="I305" t="inlineStr"/>
+      <c r="J305" t="inlineStr"/>
     </row>
     <row r="306">
       <c r="A306" t="inlineStr">
@@ -10564,6 +10893,7 @@
         </is>
       </c>
       <c r="I306" t="inlineStr"/>
+      <c r="J306" t="inlineStr"/>
     </row>
     <row r="307">
       <c r="A307" t="inlineStr">
@@ -10597,6 +10927,7 @@
         </is>
       </c>
       <c r="I307" t="inlineStr"/>
+      <c r="J307" t="inlineStr"/>
     </row>
     <row r="308">
       <c r="A308" t="inlineStr">
@@ -10630,6 +10961,7 @@
         </is>
       </c>
       <c r="I308" t="inlineStr"/>
+      <c r="J308" t="inlineStr"/>
     </row>
     <row r="309">
       <c r="A309" t="inlineStr">
@@ -10663,6 +10995,7 @@
         </is>
       </c>
       <c r="I309" t="inlineStr"/>
+      <c r="J309" t="inlineStr"/>
     </row>
     <row r="310">
       <c r="A310" t="inlineStr">
@@ -10696,6 +11029,7 @@
         </is>
       </c>
       <c r="I310" t="inlineStr"/>
+      <c r="J310" t="inlineStr"/>
     </row>
     <row r="311">
       <c r="A311" t="inlineStr">
@@ -10729,6 +11063,7 @@
         </is>
       </c>
       <c r="I311" t="inlineStr"/>
+      <c r="J311" t="inlineStr"/>
     </row>
     <row r="312">
       <c r="A312" t="inlineStr">
@@ -10746,10 +11081,15 @@
           <t>CNoR</t>
         </is>
       </c>
-      <c r="F312" t="inlineStr"/>
+      <c r="F312" t="inlineStr">
+        <is>
+          <t>Resolved - using original data (no GIS coverage)</t>
+        </is>
+      </c>
       <c r="G312" t="inlineStr"/>
       <c r="H312" t="inlineStr"/>
       <c r="I312" t="inlineStr"/>
+      <c r="J312" t="inlineStr"/>
     </row>
     <row r="313">
       <c r="A313" t="inlineStr">
@@ -10783,6 +11123,7 @@
         </is>
       </c>
       <c r="I313" t="inlineStr"/>
+      <c r="J313" t="inlineStr"/>
     </row>
     <row r="314">
       <c r="A314" t="inlineStr">
@@ -10816,6 +11157,7 @@
         </is>
       </c>
       <c r="I314" t="inlineStr"/>
+      <c r="J314" t="inlineStr"/>
     </row>
     <row r="315">
       <c r="A315" t="inlineStr">
@@ -10849,6 +11191,7 @@
         </is>
       </c>
       <c r="I315" t="inlineStr"/>
+      <c r="J315" t="inlineStr"/>
     </row>
     <row r="316">
       <c r="A316" t="inlineStr">
@@ -10882,6 +11225,7 @@
         </is>
       </c>
       <c r="I316" t="inlineStr"/>
+      <c r="J316" t="inlineStr"/>
     </row>
     <row r="317">
       <c r="A317" t="inlineStr">
@@ -10915,6 +11259,7 @@
         </is>
       </c>
       <c r="I317" t="inlineStr"/>
+      <c r="J317" t="inlineStr"/>
     </row>
     <row r="318">
       <c r="A318" t="inlineStr">
@@ -10948,6 +11293,7 @@
         </is>
       </c>
       <c r="I318" t="inlineStr"/>
+      <c r="J318" t="inlineStr"/>
     </row>
     <row r="319">
       <c r="A319" t="inlineStr">
@@ -10964,18 +11310,14 @@
         </is>
       </c>
       <c r="D319" t="n">
-        <v>1909</v>
+        <v>1906</v>
       </c>
       <c r="E319" t="inlineStr">
         <is>
-          <t>CPR or CNoR (unclear)</t>
-        </is>
-      </c>
-      <c r="F319" t="inlineStr">
-        <is>
-          <t>Year: 1909 vs 1906 (-3); Missing in GIS: CPR</t>
-        </is>
-      </c>
+          <t>CNoR</t>
+        </is>
+      </c>
+      <c r="F319" t="inlineStr"/>
       <c r="G319" t="n">
         <v>1906</v>
       </c>
@@ -10984,11 +11326,8 @@
           <t>CNoR</t>
         </is>
       </c>
-      <c r="I319" t="inlineStr">
-        <is>
-          <t>CPR: VERY LOW - nearest line 136km away</t>
-        </is>
-      </c>
+      <c r="I319" t="inlineStr"/>
+      <c r="J319" t="inlineStr"/>
     </row>
     <row r="320">
       <c r="A320" t="inlineStr">
@@ -11022,6 +11361,7 @@
         </is>
       </c>
       <c r="I320" t="inlineStr"/>
+      <c r="J320" t="inlineStr"/>
     </row>
     <row r="321">
       <c r="A321" t="inlineStr">
@@ -11055,6 +11395,7 @@
         </is>
       </c>
       <c r="I321" t="inlineStr"/>
+      <c r="J321" t="inlineStr"/>
     </row>
     <row r="322">
       <c r="A322" t="inlineStr">
@@ -11071,7 +11412,7 @@
         </is>
       </c>
       <c r="D322" t="n">
-        <v>1908</v>
+        <v>1882</v>
       </c>
       <c r="E322" t="inlineStr">
         <is>
@@ -11080,7 +11421,7 @@
       </c>
       <c r="F322" t="inlineStr">
         <is>
-          <t>Year: 1908 vs 1882 (-26)</t>
+          <t>Resolved - GIS date, original railway context kept</t>
         </is>
       </c>
       <c r="G322" t="n">
@@ -11092,6 +11433,7 @@
         </is>
       </c>
       <c r="I322" t="inlineStr"/>
+      <c r="J322" t="inlineStr"/>
     </row>
     <row r="323">
       <c r="A323" t="inlineStr">
@@ -11125,6 +11467,7 @@
         </is>
       </c>
       <c r="I323" t="inlineStr"/>
+      <c r="J323" t="inlineStr"/>
     </row>
     <row r="324">
       <c r="A324" t="inlineStr">
@@ -11158,6 +11501,7 @@
         </is>
       </c>
       <c r="I324" t="inlineStr"/>
+      <c r="J324" t="inlineStr"/>
     </row>
     <row r="325">
       <c r="A325" t="inlineStr">
@@ -11191,6 +11535,7 @@
         </is>
       </c>
       <c r="I325" t="inlineStr"/>
+      <c r="J325" t="inlineStr"/>
     </row>
     <row r="326">
       <c r="A326" t="inlineStr">
@@ -11224,6 +11569,7 @@
         </is>
       </c>
       <c r="I326" t="inlineStr"/>
+      <c r="J326" t="inlineStr"/>
     </row>
     <row r="327">
       <c r="A327" t="inlineStr">
@@ -11257,6 +11603,7 @@
         </is>
       </c>
       <c r="I327" t="inlineStr"/>
+      <c r="J327" t="inlineStr"/>
     </row>
     <row r="328">
       <c r="A328" t="inlineStr">
@@ -11290,6 +11637,7 @@
         </is>
       </c>
       <c r="I328" t="inlineStr"/>
+      <c r="J328" t="inlineStr"/>
     </row>
     <row r="329">
       <c r="A329" t="inlineStr">
@@ -11323,6 +11671,7 @@
         </is>
       </c>
       <c r="I329" t="inlineStr"/>
+      <c r="J329" t="inlineStr"/>
     </row>
     <row r="330">
       <c r="A330" t="inlineStr">
@@ -11356,6 +11705,7 @@
         </is>
       </c>
       <c r="I330" t="inlineStr"/>
+      <c r="J330" t="inlineStr"/>
     </row>
     <row r="331">
       <c r="A331" t="inlineStr">
@@ -11389,6 +11739,7 @@
         </is>
       </c>
       <c r="I331" t="inlineStr"/>
+      <c r="J331" t="inlineStr"/>
     </row>
     <row r="332">
       <c r="A332" t="inlineStr">
@@ -11422,6 +11773,7 @@
         </is>
       </c>
       <c r="I332" t="inlineStr"/>
+      <c r="J332" t="inlineStr"/>
     </row>
     <row r="333">
       <c r="A333" t="inlineStr">
@@ -11439,10 +11791,15 @@
           <t>CPR (date is for Wynyard, as no specific date available for Kandahar)</t>
         </is>
       </c>
-      <c r="F333" t="inlineStr"/>
+      <c r="F333" t="inlineStr">
+        <is>
+          <t>Resolved - using original data (no GIS coverage)</t>
+        </is>
+      </c>
       <c r="G333" t="inlineStr"/>
       <c r="H333" t="inlineStr"/>
       <c r="I333" t="inlineStr"/>
+      <c r="J333" t="inlineStr"/>
     </row>
     <row r="334">
       <c r="A334" t="inlineStr">
@@ -11476,6 +11833,7 @@
         </is>
       </c>
       <c r="I334" t="inlineStr"/>
+      <c r="J334" t="inlineStr"/>
     </row>
     <row r="335">
       <c r="A335" t="inlineStr">
@@ -11509,6 +11867,7 @@
         </is>
       </c>
       <c r="I335" t="inlineStr"/>
+      <c r="J335" t="inlineStr"/>
     </row>
     <row r="336">
       <c r="A336" t="inlineStr">
@@ -11542,6 +11901,7 @@
         </is>
       </c>
       <c r="I336" t="inlineStr"/>
+      <c r="J336" t="inlineStr"/>
     </row>
     <row r="337">
       <c r="A337" t="inlineStr">
@@ -11575,6 +11935,7 @@
         </is>
       </c>
       <c r="I337" t="inlineStr"/>
+      <c r="J337" t="inlineStr"/>
     </row>
     <row r="338">
       <c r="A338" t="inlineStr">
@@ -11608,6 +11969,7 @@
         </is>
       </c>
       <c r="I338" t="inlineStr"/>
+      <c r="J338" t="inlineStr"/>
     </row>
     <row r="339">
       <c r="A339" t="inlineStr">
@@ -11641,6 +12003,7 @@
         </is>
       </c>
       <c r="I339" t="inlineStr"/>
+      <c r="J339" t="inlineStr"/>
     </row>
     <row r="340">
       <c r="A340" t="inlineStr">
@@ -11674,6 +12037,7 @@
         </is>
       </c>
       <c r="I340" t="inlineStr"/>
+      <c r="J340" t="inlineStr"/>
     </row>
     <row r="341">
       <c r="A341" t="inlineStr">
@@ -11707,6 +12071,7 @@
         </is>
       </c>
       <c r="I341" t="inlineStr"/>
+      <c r="J341" t="inlineStr"/>
     </row>
     <row r="342">
       <c r="A342" t="inlineStr">
@@ -11740,6 +12105,7 @@
         </is>
       </c>
       <c r="I342" t="inlineStr"/>
+      <c r="J342" t="inlineStr"/>
     </row>
     <row r="343">
       <c r="A343" t="inlineStr">
@@ -11773,6 +12139,7 @@
         </is>
       </c>
       <c r="I343" t="inlineStr"/>
+      <c r="J343" t="inlineStr"/>
     </row>
     <row r="344">
       <c r="A344" t="inlineStr">
@@ -11806,6 +12173,7 @@
         </is>
       </c>
       <c r="I344" t="inlineStr"/>
+      <c r="J344" t="inlineStr"/>
     </row>
     <row r="345">
       <c r="A345" t="inlineStr">
@@ -11839,6 +12207,7 @@
         </is>
       </c>
       <c r="I345" t="inlineStr"/>
+      <c r="J345" t="inlineStr"/>
     </row>
     <row r="346">
       <c r="A346" t="inlineStr">
@@ -11872,6 +12241,7 @@
         </is>
       </c>
       <c r="I346" t="inlineStr"/>
+      <c r="J346" t="inlineStr"/>
     </row>
     <row r="347">
       <c r="A347" t="inlineStr">
@@ -11905,6 +12275,7 @@
         </is>
       </c>
       <c r="I347" t="inlineStr"/>
+      <c r="J347" t="inlineStr"/>
     </row>
     <row r="348">
       <c r="A348" t="inlineStr">
@@ -11922,7 +12293,11 @@
           <t>CPR</t>
         </is>
       </c>
-      <c r="F348" t="inlineStr"/>
+      <c r="F348" t="inlineStr">
+        <is>
+          <t>Resolved - using original data (no GIS coverage)</t>
+        </is>
+      </c>
       <c r="G348" t="n">
         <v>1911</v>
       </c>
@@ -11932,6 +12307,7 @@
         </is>
       </c>
       <c r="I348" t="inlineStr"/>
+      <c r="J348" t="inlineStr"/>
     </row>
     <row r="349">
       <c r="A349" t="inlineStr">
@@ -11965,6 +12341,7 @@
         </is>
       </c>
       <c r="I349" t="inlineStr"/>
+      <c r="J349" t="inlineStr"/>
     </row>
     <row r="350">
       <c r="A350" t="inlineStr">
@@ -11998,6 +12375,7 @@
         </is>
       </c>
       <c r="I350" t="inlineStr"/>
+      <c r="J350" t="inlineStr"/>
     </row>
     <row r="351">
       <c r="A351" t="inlineStr">
@@ -12031,6 +12409,7 @@
         </is>
       </c>
       <c r="I351" t="inlineStr"/>
+      <c r="J351" t="inlineStr"/>
     </row>
     <row r="352">
       <c r="A352" t="inlineStr">
@@ -12064,6 +12443,7 @@
         </is>
       </c>
       <c r="I352" t="inlineStr"/>
+      <c r="J352" t="inlineStr"/>
     </row>
     <row r="353">
       <c r="A353" t="inlineStr">
@@ -12097,6 +12477,7 @@
         </is>
       </c>
       <c r="I353" t="inlineStr"/>
+      <c r="J353" t="inlineStr"/>
     </row>
     <row r="354">
       <c r="A354" t="inlineStr">
@@ -12130,6 +12511,7 @@
         </is>
       </c>
       <c r="I354" t="inlineStr"/>
+      <c r="J354" t="inlineStr"/>
     </row>
     <row r="355">
       <c r="A355" t="inlineStr">
@@ -12163,6 +12545,7 @@
         </is>
       </c>
       <c r="I355" t="inlineStr"/>
+      <c r="J355" t="inlineStr"/>
     </row>
     <row r="356">
       <c r="A356" t="inlineStr">
@@ -12196,6 +12579,7 @@
         </is>
       </c>
       <c r="I356" t="inlineStr"/>
+      <c r="J356" t="inlineStr"/>
     </row>
     <row r="357">
       <c r="A357" t="inlineStr">
@@ -12229,6 +12613,7 @@
         </is>
       </c>
       <c r="I357" t="inlineStr"/>
+      <c r="J357" t="inlineStr"/>
     </row>
     <row r="358">
       <c r="A358" t="inlineStr">
@@ -12262,6 +12647,7 @@
         </is>
       </c>
       <c r="I358" t="inlineStr"/>
+      <c r="J358" t="inlineStr"/>
     </row>
     <row r="359">
       <c r="A359" t="inlineStr">
@@ -12295,6 +12681,7 @@
         </is>
       </c>
       <c r="I359" t="inlineStr"/>
+      <c r="J359" t="inlineStr"/>
     </row>
     <row r="360">
       <c r="A360" t="inlineStr">
@@ -12328,6 +12715,7 @@
         </is>
       </c>
       <c r="I360" t="inlineStr"/>
+      <c r="J360" t="inlineStr"/>
     </row>
     <row r="361">
       <c r="A361" t="inlineStr">
@@ -12345,7 +12733,11 @@
           <t>CNoR</t>
         </is>
       </c>
-      <c r="F361" t="inlineStr"/>
+      <c r="F361" t="inlineStr">
+        <is>
+          <t>Resolved - using original data (no GIS coverage)</t>
+        </is>
+      </c>
       <c r="G361" t="n">
         <v>1911</v>
       </c>
@@ -12355,6 +12747,7 @@
         </is>
       </c>
       <c r="I361" t="inlineStr"/>
+      <c r="J361" t="inlineStr"/>
     </row>
     <row r="362">
       <c r="A362" t="inlineStr">
@@ -12388,6 +12781,7 @@
         </is>
       </c>
       <c r="I362" t="inlineStr"/>
+      <c r="J362" t="inlineStr"/>
     </row>
     <row r="363">
       <c r="A363" t="inlineStr">
@@ -12421,6 +12815,7 @@
         </is>
       </c>
       <c r="I363" t="inlineStr"/>
+      <c r="J363" t="inlineStr"/>
     </row>
     <row r="364">
       <c r="A364" t="inlineStr">
@@ -12454,6 +12849,7 @@
         </is>
       </c>
       <c r="I364" t="inlineStr"/>
+      <c r="J364" t="inlineStr"/>
     </row>
     <row r="365">
       <c r="A365" t="inlineStr">
@@ -12487,6 +12883,7 @@
         </is>
       </c>
       <c r="I365" t="inlineStr"/>
+      <c r="J365" t="inlineStr"/>
     </row>
     <row r="366">
       <c r="A366" t="inlineStr">
@@ -12520,6 +12917,7 @@
         </is>
       </c>
       <c r="I366" t="inlineStr"/>
+      <c r="J366" t="inlineStr"/>
     </row>
     <row r="367">
       <c r="A367" t="inlineStr">
@@ -12553,6 +12951,7 @@
         </is>
       </c>
       <c r="I367" t="inlineStr"/>
+      <c r="J367" t="inlineStr"/>
     </row>
     <row r="368">
       <c r="A368" t="inlineStr">
@@ -12586,6 +12985,7 @@
         </is>
       </c>
       <c r="I368" t="inlineStr"/>
+      <c r="J368" t="inlineStr"/>
     </row>
     <row r="369">
       <c r="A369" t="inlineStr">
@@ -12603,10 +13003,15 @@
           <t>CPR (date is for Wynyard, as no specific date available for Kandahar)</t>
         </is>
       </c>
-      <c r="F369" t="inlineStr"/>
+      <c r="F369" t="inlineStr">
+        <is>
+          <t>Resolved - using original data (no GIS coverage)</t>
+        </is>
+      </c>
       <c r="G369" t="inlineStr"/>
       <c r="H369" t="inlineStr"/>
       <c r="I369" t="inlineStr"/>
+      <c r="J369" t="inlineStr"/>
     </row>
     <row r="370">
       <c r="A370" t="inlineStr">
@@ -12640,6 +13045,7 @@
         </is>
       </c>
       <c r="I370" t="inlineStr"/>
+      <c r="J370" t="inlineStr"/>
     </row>
     <row r="371">
       <c r="A371" t="inlineStr">
@@ -12673,6 +13079,7 @@
         </is>
       </c>
       <c r="I371" t="inlineStr"/>
+      <c r="J371" t="inlineStr"/>
     </row>
     <row r="372">
       <c r="A372" t="inlineStr">
@@ -12706,6 +13113,7 @@
         </is>
       </c>
       <c r="I372" t="inlineStr"/>
+      <c r="J372" t="inlineStr"/>
     </row>
     <row r="373">
       <c r="A373" t="inlineStr">
@@ -12739,6 +13147,7 @@
         </is>
       </c>
       <c r="I373" t="inlineStr"/>
+      <c r="J373" t="inlineStr"/>
     </row>
     <row r="374">
       <c r="A374" t="inlineStr">
@@ -12772,6 +13181,7 @@
         </is>
       </c>
       <c r="I374" t="inlineStr"/>
+      <c r="J374" t="inlineStr"/>
     </row>
     <row r="375">
       <c r="A375" t="inlineStr">
@@ -12805,6 +13215,7 @@
         </is>
       </c>
       <c r="I375" t="inlineStr"/>
+      <c r="J375" t="inlineStr"/>
     </row>
     <row r="376">
       <c r="A376" t="inlineStr">
@@ -12838,6 +13249,7 @@
         </is>
       </c>
       <c r="I376" t="inlineStr"/>
+      <c r="J376" t="inlineStr"/>
     </row>
     <row r="377">
       <c r="A377" t="inlineStr">
@@ -12871,6 +13283,7 @@
         </is>
       </c>
       <c r="I377" t="inlineStr"/>
+      <c r="J377" t="inlineStr"/>
     </row>
     <row r="378">
       <c r="A378" t="inlineStr">
@@ -12904,6 +13317,7 @@
         </is>
       </c>
       <c r="I378" t="inlineStr"/>
+      <c r="J378" t="inlineStr"/>
     </row>
     <row r="379">
       <c r="A379" t="inlineStr">
@@ -12937,6 +13351,7 @@
         </is>
       </c>
       <c r="I379" t="inlineStr"/>
+      <c r="J379" t="inlineStr"/>
     </row>
     <row r="380">
       <c r="A380" t="inlineStr">
@@ -12970,6 +13385,7 @@
         </is>
       </c>
       <c r="I380" t="inlineStr"/>
+      <c r="J380" t="inlineStr"/>
     </row>
     <row r="381">
       <c r="A381" t="inlineStr">
@@ -13003,6 +13419,7 @@
         </is>
       </c>
       <c r="I381" t="inlineStr"/>
+      <c r="J381" t="inlineStr"/>
     </row>
     <row r="382">
       <c r="A382" t="inlineStr">
@@ -13036,6 +13453,7 @@
         </is>
       </c>
       <c r="I382" t="inlineStr"/>
+      <c r="J382" t="inlineStr"/>
     </row>
     <row r="383">
       <c r="A383" t="inlineStr">
@@ -13069,6 +13487,7 @@
         </is>
       </c>
       <c r="I383" t="inlineStr"/>
+      <c r="J383" t="inlineStr"/>
     </row>
     <row r="384">
       <c r="A384" t="inlineStr">
@@ -13102,6 +13521,7 @@
         </is>
       </c>
       <c r="I384" t="inlineStr"/>
+      <c r="J384" t="inlineStr"/>
     </row>
     <row r="385">
       <c r="A385" t="inlineStr">
@@ -13135,6 +13555,7 @@
         </is>
       </c>
       <c r="I385" t="inlineStr"/>
+      <c r="J385" t="inlineStr"/>
     </row>
     <row r="386">
       <c r="A386" t="inlineStr">
@@ -13168,6 +13589,7 @@
         </is>
       </c>
       <c r="I386" t="inlineStr"/>
+      <c r="J386" t="inlineStr"/>
     </row>
     <row r="387">
       <c r="A387" t="inlineStr">
@@ -13201,6 +13623,7 @@
         </is>
       </c>
       <c r="I387" t="inlineStr"/>
+      <c r="J387" t="inlineStr"/>
     </row>
     <row r="388">
       <c r="A388" t="inlineStr">
@@ -13234,6 +13657,7 @@
         </is>
       </c>
       <c r="I388" t="inlineStr"/>
+      <c r="J388" t="inlineStr"/>
     </row>
     <row r="389">
       <c r="A389" t="inlineStr">
@@ -13267,6 +13691,7 @@
         </is>
       </c>
       <c r="I389" t="inlineStr"/>
+      <c r="J389" t="inlineStr"/>
     </row>
     <row r="390">
       <c r="A390" t="inlineStr">
@@ -13300,6 +13725,7 @@
         </is>
       </c>
       <c r="I390" t="inlineStr"/>
+      <c r="J390" t="inlineStr"/>
     </row>
     <row r="391">
       <c r="A391" t="inlineStr">
@@ -13333,6 +13759,7 @@
         </is>
       </c>
       <c r="I391" t="inlineStr"/>
+      <c r="J391" t="inlineStr"/>
     </row>
     <row r="392">
       <c r="A392" t="inlineStr">
@@ -13366,6 +13793,7 @@
         </is>
       </c>
       <c r="I392" t="inlineStr"/>
+      <c r="J392" t="inlineStr"/>
     </row>
     <row r="393">
       <c r="A393" t="inlineStr">
@@ -13399,6 +13827,7 @@
         </is>
       </c>
       <c r="I393" t="inlineStr"/>
+      <c r="J393" t="inlineStr"/>
     </row>
     <row r="394">
       <c r="A394" t="inlineStr">
@@ -13432,6 +13861,7 @@
         </is>
       </c>
       <c r="I394" t="inlineStr"/>
+      <c r="J394" t="inlineStr"/>
     </row>
     <row r="395">
       <c r="A395" t="inlineStr">
@@ -13465,6 +13895,7 @@
         </is>
       </c>
       <c r="I395" t="inlineStr"/>
+      <c r="J395" t="inlineStr"/>
     </row>
     <row r="396">
       <c r="A396" t="inlineStr">
@@ -13498,6 +13929,7 @@
         </is>
       </c>
       <c r="I396" t="inlineStr"/>
+      <c r="J396" t="inlineStr"/>
     </row>
     <row r="397">
       <c r="A397" t="inlineStr">
@@ -13531,6 +13963,7 @@
         </is>
       </c>
       <c r="I397" t="inlineStr"/>
+      <c r="J397" t="inlineStr"/>
     </row>
     <row r="398">
       <c r="A398" t="inlineStr">
@@ -13564,6 +13997,7 @@
         </is>
       </c>
       <c r="I398" t="inlineStr"/>
+      <c r="J398" t="inlineStr"/>
     </row>
     <row r="399">
       <c r="A399" t="inlineStr">
@@ -13597,6 +14031,7 @@
         </is>
       </c>
       <c r="I399" t="inlineStr"/>
+      <c r="J399" t="inlineStr"/>
     </row>
     <row r="400">
       <c r="A400" t="inlineStr">
@@ -13630,6 +14065,7 @@
         </is>
       </c>
       <c r="I400" t="inlineStr"/>
+      <c r="J400" t="inlineStr"/>
     </row>
     <row r="401">
       <c r="A401" t="inlineStr">
@@ -13663,6 +14099,7 @@
         </is>
       </c>
       <c r="I401" t="inlineStr"/>
+      <c r="J401" t="inlineStr"/>
     </row>
     <row r="402">
       <c r="A402" t="inlineStr">
@@ -13696,6 +14133,7 @@
         </is>
       </c>
       <c r="I402" t="inlineStr"/>
+      <c r="J402" t="inlineStr"/>
     </row>
     <row r="403">
       <c r="A403" t="inlineStr">
@@ -13713,10 +14151,15 @@
           <t>CPR</t>
         </is>
       </c>
-      <c r="F403" t="inlineStr"/>
+      <c r="F403" t="inlineStr">
+        <is>
+          <t>Resolved - using original data (no GIS coverage)</t>
+        </is>
+      </c>
       <c r="G403" t="inlineStr"/>
       <c r="H403" t="inlineStr"/>
       <c r="I403" t="inlineStr"/>
+      <c r="J403" t="inlineStr"/>
     </row>
     <row r="404">
       <c r="A404" t="inlineStr">
@@ -13734,10 +14177,15 @@
           <t>CNoR</t>
         </is>
       </c>
-      <c r="F404" t="inlineStr"/>
+      <c r="F404" t="inlineStr">
+        <is>
+          <t>Resolved - using original data (no GIS coverage)</t>
+        </is>
+      </c>
       <c r="G404" t="inlineStr"/>
       <c r="H404" t="inlineStr"/>
       <c r="I404" t="inlineStr"/>
+      <c r="J404" t="inlineStr"/>
     </row>
     <row r="405">
       <c r="A405" t="inlineStr">
@@ -13771,6 +14219,7 @@
         </is>
       </c>
       <c r="I405" t="inlineStr"/>
+      <c r="J405" t="inlineStr"/>
     </row>
     <row r="406">
       <c r="A406" t="inlineStr">
@@ -13804,6 +14253,7 @@
         </is>
       </c>
       <c r="I406" t="inlineStr"/>
+      <c r="J406" t="inlineStr"/>
     </row>
     <row r="407">
       <c r="A407" t="inlineStr">
@@ -13837,6 +14287,7 @@
         </is>
       </c>
       <c r="I407" t="inlineStr"/>
+      <c r="J407" t="inlineStr"/>
     </row>
     <row r="408">
       <c r="A408" t="inlineStr">
@@ -13870,6 +14321,7 @@
         </is>
       </c>
       <c r="I408" t="inlineStr"/>
+      <c r="J408" t="inlineStr"/>
     </row>
     <row r="409">
       <c r="A409" t="inlineStr">
@@ -13903,6 +14355,7 @@
         </is>
       </c>
       <c r="I409" t="inlineStr"/>
+      <c r="J409" t="inlineStr"/>
     </row>
     <row r="410">
       <c r="A410" t="inlineStr">
@@ -13936,6 +14389,7 @@
         </is>
       </c>
       <c r="I410" t="inlineStr"/>
+      <c r="J410" t="inlineStr"/>
     </row>
     <row r="411">
       <c r="A411" t="inlineStr">
@@ -13969,6 +14423,7 @@
         </is>
       </c>
       <c r="I411" t="inlineStr"/>
+      <c r="J411" t="inlineStr"/>
     </row>
     <row r="412">
       <c r="A412" t="inlineStr">
@@ -13985,7 +14440,7 @@
         </is>
       </c>
       <c r="D412" t="n">
-        <v>1917</v>
+        <v>1914</v>
       </c>
       <c r="E412" t="inlineStr">
         <is>
@@ -13994,7 +14449,7 @@
       </c>
       <c r="F412" t="inlineStr">
         <is>
-          <t>Year: 1917 vs 1914 (-3)</t>
+          <t>Resolved - using GIS data</t>
         </is>
       </c>
       <c r="G412" t="n">
@@ -14006,6 +14461,7 @@
         </is>
       </c>
       <c r="I412" t="inlineStr"/>
+      <c r="J412" t="inlineStr"/>
     </row>
     <row r="413">
       <c r="A413" t="inlineStr">
@@ -14039,6 +14495,7 @@
         </is>
       </c>
       <c r="I413" t="inlineStr"/>
+      <c r="J413" t="inlineStr"/>
     </row>
     <row r="414">
       <c r="A414" t="inlineStr">
@@ -14072,6 +14529,7 @@
         </is>
       </c>
       <c r="I414" t="inlineStr"/>
+      <c r="J414" t="inlineStr"/>
     </row>
     <row r="415">
       <c r="A415" t="inlineStr">
@@ -14105,6 +14563,7 @@
         </is>
       </c>
       <c r="I415" t="inlineStr"/>
+      <c r="J415" t="inlineStr"/>
     </row>
     <row r="416">
       <c r="A416" t="inlineStr">
@@ -14138,6 +14597,7 @@
         </is>
       </c>
       <c r="I416" t="inlineStr"/>
+      <c r="J416" t="inlineStr"/>
     </row>
     <row r="417">
       <c r="A417" t="inlineStr">
@@ -14171,6 +14631,7 @@
         </is>
       </c>
       <c r="I417" t="inlineStr"/>
+      <c r="J417" t="inlineStr"/>
     </row>
     <row r="418">
       <c r="A418" t="inlineStr">
@@ -14204,6 +14665,7 @@
         </is>
       </c>
       <c r="I418" t="inlineStr"/>
+      <c r="J418" t="inlineStr"/>
     </row>
     <row r="419">
       <c r="A419" t="inlineStr">
@@ -14237,6 +14699,7 @@
         </is>
       </c>
       <c r="I419" t="inlineStr"/>
+      <c r="J419" t="inlineStr"/>
     </row>
     <row r="420">
       <c r="A420" t="inlineStr">
@@ -14270,6 +14733,7 @@
         </is>
       </c>
       <c r="I420" t="inlineStr"/>
+      <c r="J420" t="inlineStr"/>
     </row>
     <row r="421">
       <c r="A421" t="inlineStr">
@@ -14303,6 +14767,7 @@
         </is>
       </c>
       <c r="I421" t="inlineStr"/>
+      <c r="J421" t="inlineStr"/>
     </row>
     <row r="422">
       <c r="A422" t="inlineStr">
@@ -14336,6 +14801,7 @@
         </is>
       </c>
       <c r="I422" t="inlineStr"/>
+      <c r="J422" t="inlineStr"/>
     </row>
     <row r="423">
       <c r="A423" t="inlineStr">
@@ -14352,7 +14818,7 @@
         </is>
       </c>
       <c r="D423" t="n">
-        <v>1917</v>
+        <v>1914</v>
       </c>
       <c r="E423" t="inlineStr">
         <is>
@@ -14361,7 +14827,7 @@
       </c>
       <c r="F423" t="inlineStr">
         <is>
-          <t>Year: 1917 vs 1914 (-3)</t>
+          <t>Resolved - using GIS data</t>
         </is>
       </c>
       <c r="G423" t="n">
@@ -14373,6 +14839,7 @@
         </is>
       </c>
       <c r="I423" t="inlineStr"/>
+      <c r="J423" t="inlineStr"/>
     </row>
     <row r="424">
       <c r="A424" t="inlineStr">
@@ -14406,6 +14873,7 @@
         </is>
       </c>
       <c r="I424" t="inlineStr"/>
+      <c r="J424" t="inlineStr"/>
     </row>
     <row r="425">
       <c r="A425" t="inlineStr">
@@ -14423,10 +14891,15 @@
           <t>CPR</t>
         </is>
       </c>
-      <c r="F425" t="inlineStr"/>
+      <c r="F425" t="inlineStr">
+        <is>
+          <t>Resolved - using original data (no GIS coverage)</t>
+        </is>
+      </c>
       <c r="G425" t="inlineStr"/>
       <c r="H425" t="inlineStr"/>
       <c r="I425" t="inlineStr"/>
+      <c r="J425" t="inlineStr"/>
     </row>
     <row r="426">
       <c r="A426" t="inlineStr">
@@ -14460,6 +14933,7 @@
         </is>
       </c>
       <c r="I426" t="inlineStr"/>
+      <c r="J426" t="inlineStr"/>
     </row>
     <row r="427">
       <c r="A427" t="inlineStr">
@@ -14493,6 +14967,7 @@
         </is>
       </c>
       <c r="I427" t="inlineStr"/>
+      <c r="J427" t="inlineStr"/>
     </row>
     <row r="428">
       <c r="A428" t="inlineStr">
@@ -14526,6 +15001,7 @@
         </is>
       </c>
       <c r="I428" t="inlineStr"/>
+      <c r="J428" t="inlineStr"/>
     </row>
     <row r="429">
       <c r="A429" t="inlineStr">
@@ -14559,6 +15035,7 @@
         </is>
       </c>
       <c r="I429" t="inlineStr"/>
+      <c r="J429" t="inlineStr"/>
     </row>
     <row r="430">
       <c r="A430" t="inlineStr">
@@ -14592,6 +15069,7 @@
         </is>
       </c>
       <c r="I430" t="inlineStr"/>
+      <c r="J430" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>